<commit_message>
Some classes werer refactored, flash_module added
</commit_message>
<xml_diff>
--- a/data/teste.xlsx
+++ b/data/teste.xlsx
@@ -396,15 +396,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N109"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81:J95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="12.44140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,3349 +483,2698 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>288.15</v>
+        <v>429.9</v>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>74.91</v>
       </c>
       <c r="D2" t="n">
-        <v>1.191895113230036</v>
+        <v>2.14642</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8464677335995328</v>
+        <v>0.02564537360717186</v>
       </c>
       <c r="F2" t="n">
-        <v>1.181379939608075</v>
+        <v>38.99338786471588</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8479473118770369</v>
+        <v>0.05374613322224337</v>
       </c>
       <c r="H2" t="n">
-        <v>0.008822230668825162</v>
+        <v>17.16670915511218</v>
       </c>
       <c r="M2" t="n">
-        <v>1.023785891666495e-06</v>
+        <v>15.60573610141844</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>288.15</v>
+        <v>447.82</v>
       </c>
       <c r="C3" t="n">
-        <v>29.5</v>
+        <v>78.44</v>
       </c>
       <c r="D3" t="n">
-        <v>1.533742331288344</v>
+        <v>2.14448</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6563574710771028</v>
+        <v>0.2391172820196638</v>
       </c>
       <c r="F3" t="n">
-        <v>1.523560017316431</v>
+        <v>4.182048204770767</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8081829184869478</v>
+        <v>0.5037451837569101</v>
       </c>
       <c r="H3" t="n">
-        <v>0.006638868709686729</v>
+        <v>0.950145585303088</v>
       </c>
       <c r="M3" t="n">
-        <v>9.599955353944221e-07</v>
+        <v>0.04772050792060648</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>288.15</v>
+        <v>465.84</v>
       </c>
       <c r="C4" t="n">
-        <v>33.3</v>
+        <v>81.98</v>
       </c>
       <c r="D4" t="n">
-        <v>1.795332136445242</v>
+        <v>2.1425</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5605182135645552</v>
+        <v>0.2284628913652686</v>
       </c>
       <c r="F4" t="n">
-        <v>1.78406334673874</v>
+        <v>4.377078456917499</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7790784306925808</v>
+        <v>0.4835625372877853</v>
       </c>
       <c r="H4" t="n">
-        <v>0.006276715866521876</v>
+        <v>1.042977109413068</v>
       </c>
       <c r="M4" t="n">
-        <v>1.175792791197926e-06</v>
+        <v>0.05739472275999761</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>288.15</v>
+        <v>483.68</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>85.48</v>
       </c>
       <c r="D5" t="n">
-        <v>2.403846153846154</v>
+        <v>2.14052</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4175444486538161</v>
+        <v>0.2184577456126565</v>
       </c>
       <c r="F5" t="n">
-        <v>2.394954604770939</v>
+        <v>4.577544262372284</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7145519172215039</v>
+        <v>0.4643438236581038</v>
       </c>
       <c r="H5" t="n">
-        <v>0.003698884415289186</v>
+        <v>1.13851973463097</v>
       </c>
       <c r="M5" t="n">
-        <v>7.320337496013506e-07</v>
+        <v>0.06826537075162273</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>288.15</v>
+        <v>500.99</v>
       </c>
       <c r="C6" t="n">
-        <v>48.7</v>
+        <v>88.87</v>
       </c>
       <c r="D6" t="n">
-        <v>3.184713375796179</v>
+        <v>2.13857</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3140048183310324</v>
+        <v>0.2274636039128339</v>
       </c>
       <c r="F6" t="n">
-        <v>3.184664507108845</v>
+        <v>4.396307729227789</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6382818447670923</v>
+        <v>0.4852928365781342</v>
       </c>
       <c r="H6" t="n">
-        <v>1.534476782263283e-05</v>
+        <v>1.0557230903023</v>
       </c>
       <c r="M6" t="n">
-        <v>2.211248705252373e-11</v>
+        <v>0.05859057073538683</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0,0580;0,9420</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>288.15</v>
+        <v>518.4</v>
       </c>
       <c r="C7" t="n">
-        <v>52.5</v>
+        <v>92.23999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>3.703703703703703</v>
+        <v>2.1366</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2705070723024637</v>
+        <v>0.2768849537623453</v>
       </c>
       <c r="F7" t="n">
-        <v>3.696761018070033</v>
+        <v>3.611608310281518</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5927685389991191</v>
+        <v>0.5925424921896478</v>
       </c>
       <c r="H7" t="n">
-        <v>0.001874525121090858</v>
+        <v>0.6903530423483655</v>
       </c>
       <c r="M7" t="n">
-        <v>4.463044797033854e-07</v>
+        <v>0.02500746569424757</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>288.15</v>
+        <v>535.55</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>95.54000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>1.186239620403321</v>
+        <v>2.13463</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8516450691558848</v>
+        <v>0.3004522147012968</v>
       </c>
       <c r="F8" t="n">
-        <v>1.174198074076984</v>
+        <v>3.328316288146448</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8531336971265083</v>
+        <v>0.6446536781785528</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0101510235531023</v>
+        <v>0.5592005584791969</v>
       </c>
       <c r="M8" t="n">
-        <v>1.342581832678945e-06</v>
+        <v>0.01637801097136603</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>288.15</v>
+        <v>553.34</v>
       </c>
       <c r="C9" t="n">
-        <v>29.5</v>
+        <v>98.95999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>1.524390243902439</v>
+        <v>2.13258</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6620148364442693</v>
+        <v>0.3180683794624712</v>
       </c>
       <c r="F9" t="n">
-        <v>1.51054016458464</v>
+        <v>3.143978039219046</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8151489183496147</v>
+        <v>0.6841541395516835</v>
       </c>
       <c r="H9" t="n">
-        <v>0.009085652032476233</v>
+        <v>0.474260304053797</v>
       </c>
       <c r="M9" t="n">
-        <v>1.776154602864142e-06</v>
+        <v>0.01175777004294404</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>288.15</v>
+        <v>571.25</v>
       </c>
       <c r="C10" t="n">
-        <v>33.3</v>
+        <v>102.41</v>
       </c>
       <c r="D10" t="n">
-        <v>1.779359430604982</v>
+        <v>2.13049</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5665874756428126</v>
+        <v>0.331984492132223</v>
       </c>
       <c r="F10" t="n">
-        <v>1.764952532467235</v>
+        <v>3.012188893455058</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7875142514401723</v>
+        <v>0.7158133474192939</v>
       </c>
       <c r="H10" t="n">
-        <v>0.008096676753413804</v>
+        <v>0.4138479380119398</v>
       </c>
       <c r="M10" t="n">
-        <v>1.921839943994606e-06</v>
+        <v>0.008935551019768655</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>288.15</v>
+        <v>589.36</v>
       </c>
       <c r="C11" t="n">
-        <v>41</v>
+        <v>106.02</v>
       </c>
       <c r="D11" t="n">
-        <v>2.358490566037736</v>
+        <v>2.12835</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4247784147609371</v>
+        <v>0.3430046457822977</v>
       </c>
       <c r="F11" t="n">
-        <v>2.354168585903298</v>
+        <v>2.915412407080608</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7269315437920976</v>
+        <v>0.7421180373993548</v>
       </c>
       <c r="H11" t="n">
-        <v>0.001832519577001555</v>
+        <v>0.3697993314448322</v>
       </c>
       <c r="M11" t="n">
-        <v>1.7295844705994e-07</v>
+        <v>0.007120313018845074</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>288.15</v>
+        <v>607.33</v>
       </c>
       <c r="C12" t="n">
-        <v>48.7</v>
+        <v>109.44</v>
       </c>
       <c r="D12" t="n">
-        <v>3.08641975308642</v>
+        <v>2.12622</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3233286852038477</v>
+        <v>0.3529484569992812</v>
       </c>
       <c r="F12" t="n">
-        <v>3.092827966592368</v>
+        <v>2.8332748880725</v>
       </c>
       <c r="G12" t="n">
-        <v>0.6572345951725632</v>
+        <v>0.7649419518952109</v>
       </c>
       <c r="H12" t="n">
-        <v>0.002076261175927152</v>
+        <v>0.3325407944956307</v>
       </c>
       <c r="M12" t="n">
-        <v>3.802333364612443e-07</v>
+        <v>0.005746282928128912</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0,0980;0,9020</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>288.15</v>
+        <v>625.37</v>
       </c>
       <c r="C13" t="n">
-        <v>56.3</v>
+        <v>112.86</v>
       </c>
       <c r="D13" t="n">
-        <v>4.098360655737705</v>
+        <v>2.12406</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2430549793121907</v>
+        <v>0.3616336967248963</v>
       </c>
       <c r="F13" t="n">
-        <v>4.114295468580197</v>
+        <v>2.765229039927451</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5711630914222505</v>
+        <v>0.7849423030199673</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00388809433356818</v>
+        <v>0.3018601357435528</v>
       </c>
       <c r="M13" t="n">
-        <v>2.351095003011715e-06</v>
+        <v>0.004725261353580333</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>288.15</v>
+        <v>643.54</v>
       </c>
       <c r="C14" t="n">
-        <v>24</v>
+        <v>116.29</v>
       </c>
       <c r="D14" t="n">
-        <v>1.164144353899884</v>
+        <v>2.12186</v>
       </c>
       <c r="E14" t="n">
-        <v>0.856567868877481</v>
+        <v>0.3693592850408768</v>
       </c>
       <c r="F14" t="n">
-        <v>1.16744981493467</v>
+        <v>2.707390988937317</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8580651016268144</v>
+        <v>0.802752537857978</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00283939102888157</v>
+        <v>0.2759517540918424</v>
       </c>
       <c r="M14" t="n">
-        <v>1.011673393749221e-07</v>
+        <v>0.003940764816159911</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>288.15</v>
+        <v>661.85</v>
       </c>
       <c r="C15" t="n">
-        <v>29.5</v>
+        <v>119.76</v>
       </c>
       <c r="D15" t="n">
-        <v>1.499250374812594</v>
+        <v>2.11964</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6673616233035538</v>
+        <v>0.3762003987305971</v>
       </c>
       <c r="F15" t="n">
-        <v>1.498437975875552</v>
+        <v>2.65815773554274</v>
       </c>
       <c r="G15" t="n">
-        <v>0.8217324981805458</v>
+        <v>0.8187235969768808</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0005418700910064901</v>
+        <v>0.25406094220846</v>
       </c>
       <c r="M15" t="n">
-        <v>6.111037341719398e-09</v>
+        <v>0.003333348867748053</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>288.15</v>
+        <v>680.15</v>
       </c>
       <c r="C16" t="n">
-        <v>37.2</v>
+        <v>123.2</v>
       </c>
       <c r="D16" t="n">
-        <v>2.012072434607646</v>
+        <v>2.1174</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4941356040218387</v>
+        <v>0.3824092155256301</v>
       </c>
       <c r="F16" t="n">
-        <v>2.023735978263578</v>
+        <v>2.614999742162273</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7672489544220382</v>
+        <v>0.8331058749238608</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00579678119699855</v>
+        <v>0.2350050732796229</v>
       </c>
       <c r="M16" t="n">
-        <v>1.259613431609702e-06</v>
+        <v>0.00284604026896507</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,076;0,924</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>288.15</v>
+        <v>698.4299999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>44.8</v>
+        <v>126.61</v>
       </c>
       <c r="D17" t="n">
-        <v>2.617801047120419</v>
+        <v>2.11515</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3784971616344098</v>
+        <v>0.3880849742851603</v>
       </c>
       <c r="F17" t="n">
-        <v>2.642027738548538</v>
+        <v>2.57675526305023</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7077630065585111</v>
+        <v>0.8461313637834249</v>
       </c>
       <c r="H17" t="n">
-        <v>0.009254596125541397</v>
+        <v>0.2182376016122873</v>
       </c>
       <c r="M17" t="n">
-        <v>5.434560903271176e-06</v>
+        <v>0.00244918872270887</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>288.15</v>
+        <v>465.95</v>
       </c>
       <c r="C18" t="n">
-        <v>52.5</v>
+        <v>89.58</v>
       </c>
       <c r="D18" t="n">
-        <v>3.378378378378379</v>
+        <v>2.39629</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2913199392951187</v>
+        <v>0.1953870461124477</v>
       </c>
       <c r="F18" t="n">
-        <v>3.432652095217418</v>
+        <v>5.118046563969687</v>
       </c>
       <c r="G18" t="n">
-        <v>0.6383762662005149</v>
+        <v>0.4517866058983955</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01606502018435555</v>
+        <v>1.135821024988498</v>
       </c>
       <c r="M18" t="n">
-        <v>2.72744105511499e-05</v>
+        <v>0.08514895164956413</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0,1370;0,8630</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>288.15</v>
+        <v>483.8</v>
       </c>
       <c r="C19" t="n">
-        <v>60.2</v>
+        <v>93.97</v>
       </c>
       <c r="D19" t="n">
-        <v>4.405286343612334</v>
+        <v>2.39407</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2193264568470633</v>
+        <v>0.2199986704418683</v>
       </c>
       <c r="F19" t="n">
-        <v>4.559413462358997</v>
+        <v>4.545482015829895</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5511054833080188</v>
+        <v>0.5139362614791293</v>
       </c>
       <c r="H19" t="n">
-        <v>0.03498685595549252</v>
+        <v>0.898642068038902</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0002199552660476665</v>
+        <v>0.05320199611330172</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0,1670;0,8330</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>288.15</v>
+        <v>501.2</v>
       </c>
       <c r="C20" t="n">
-        <v>81.90000000000001</v>
+        <v>97.98</v>
       </c>
       <c r="D20" t="n">
-        <v>12.18026796589525</v>
+        <v>2.39188</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07105130355498553</v>
+        <v>0.2548290437554858</v>
       </c>
       <c r="F20" t="n">
-        <v>14.07433713339425</v>
+        <v>3.924199476098661</v>
       </c>
       <c r="G20" t="n">
-        <v>0.242886384405061</v>
+        <v>0.5991576922354199</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1555030786516682</v>
+        <v>0.6406339264924081</v>
       </c>
       <c r="M20" t="n">
-        <v>0.03321757417842933</v>
+        <v>0.02698853996357788</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0,1670;0,8330</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>288.15</v>
+        <v>518.49</v>
       </c>
       <c r="C21" t="n">
-        <v>89.59999999999999</v>
+        <v>101.8</v>
       </c>
       <c r="D21" t="n">
-        <v>14.47178002894356</v>
+        <v>2.38969</v>
       </c>
       <c r="E21" t="n">
-        <v>0.06608937631020585</v>
+        <v>0.2751724600524719</v>
       </c>
       <c r="F21" t="n">
-        <v>15.13102492155876</v>
+        <v>3.63408460210485</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2471649482226166</v>
+        <v>0.6497977478771416</v>
       </c>
       <c r="H21" t="n">
-        <v>0.04555382207971036</v>
+        <v>0.5207347405332283</v>
       </c>
       <c r="M21" t="n">
-        <v>0.004024109522585438</v>
+        <v>0.01779905661778952</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0,1670;0,8330</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>288.15</v>
+        <v>535.74</v>
       </c>
       <c r="C22" t="n">
-        <v>104.8</v>
+        <v>105.6</v>
       </c>
       <c r="D22" t="n">
-        <v>16.33986928104575</v>
+        <v>2.38747</v>
       </c>
       <c r="E22" t="n">
-        <v>0.06072265468086677</v>
+        <v>0.290073060207196</v>
       </c>
       <c r="F22" t="n">
-        <v>16.46831821262736</v>
+        <v>3.447407350705753</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2656190692582281</v>
+        <v>0.6876747583959628</v>
       </c>
       <c r="H22" t="n">
-        <v>0.007861074612794245</v>
+        <v>0.4439583955843437</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0001527697039301474</v>
+        <v>0.01291341594736931</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0,1670;0,8330</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>288.15</v>
+        <v>553.22</v>
       </c>
       <c r="C23" t="n">
-        <v>124.1</v>
+        <v>109.48</v>
       </c>
       <c r="D23" t="n">
-        <v>17.6056338028169</v>
+        <v>2.38521</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05679144441939094</v>
+        <v>0.3019174327057492</v>
       </c>
       <c r="F23" t="n">
-        <v>17.6082860758963</v>
+        <v>3.312163829157248</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2941723935313054</v>
+        <v>0.718606180832854</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0001506491109096345</v>
+        <v>0.3886256678268364</v>
       </c>
       <c r="M23" t="n">
-        <v>6.51347452563268e-08</v>
+        <v>0.009876360935509025</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0,1670;0,8330</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>288.15</v>
+        <v>571.21</v>
       </c>
       <c r="C24" t="n">
-        <v>143.4</v>
+        <v>113.4</v>
       </c>
       <c r="D24" t="n">
-        <v>18.31501831501831</v>
+        <v>2.38286</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05416923132630762</v>
+        <v>0.3122291892351855</v>
       </c>
       <c r="F24" t="n">
-        <v>18.46066439407539</v>
+        <v>3.202775507471064</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3242268987835159</v>
+        <v>0.745515360430809</v>
       </c>
       <c r="H24" t="n">
-        <v>0.007952275916516189</v>
+        <v>0.3440888291679174</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0001964146328212886</v>
+        <v>0.007727142981511862</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>288.15</v>
+        <v>589.24</v>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>117.32</v>
       </c>
       <c r="D25" t="n">
-        <v>1.166861143523921</v>
+        <v>2.38048</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8614935165920423</v>
+        <v>0.3209882769579533</v>
       </c>
       <c r="F25" t="n">
-        <v>1.160774841296394</v>
+        <v>3.115378572317741</v>
       </c>
       <c r="G25" t="n">
-        <v>0.8629993590982178</v>
+        <v>0.768661000721756</v>
       </c>
       <c r="H25" t="n">
-        <v>0.005215961008990674</v>
+        <v>0.3087186501536415</v>
       </c>
       <c r="M25" t="n">
-        <v>3.429914333777835e-07</v>
+        <v>0.006207769098789119</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>288.15</v>
+        <v>607.1</v>
       </c>
       <c r="C26" t="n">
-        <v>29.5</v>
+        <v>121.29</v>
       </c>
       <c r="D26" t="n">
-        <v>1.488095238095238</v>
+        <v>2.37811</v>
       </c>
       <c r="E26" t="n">
-        <v>0.672681589219134</v>
+        <v>0.3281572648924129</v>
       </c>
       <c r="F26" t="n">
-        <v>1.486587437543557</v>
+        <v>3.047319401348168</v>
       </c>
       <c r="G26" t="n">
-        <v>0.8282830529763177</v>
+        <v>0.7885198461230367</v>
       </c>
       <c r="H26" t="n">
-        <v>0.001013241970729695</v>
+        <v>0.2814038885283559</v>
       </c>
       <c r="M26" t="n">
-        <v>2.105057873749824e-08</v>
+        <v>0.005147600262675562</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>288.15</v>
+        <v>625.17</v>
       </c>
       <c r="C27" t="n">
-        <v>37.2</v>
+        <v>125.18</v>
       </c>
       <c r="D27" t="n">
-        <v>1.988071570576541</v>
+        <v>2.37569</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5001799541935227</v>
+        <v>0.3349027301046696</v>
       </c>
       <c r="F27" t="n">
-        <v>1.999280442200796</v>
+        <v>2.985941618593144</v>
       </c>
       <c r="G27" t="n">
-        <v>0.7766340732267546</v>
+        <v>0.8065315256536112</v>
       </c>
       <c r="H27" t="n">
-        <v>0.005638062427000427</v>
+        <v>0.2568734214451985</v>
       </c>
       <c r="M27" t="n">
-        <v>1.163322250824409e-06</v>
+        <v>0.004280540666615537</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>288.15</v>
+        <v>643.25</v>
       </c>
       <c r="C28" t="n">
-        <v>44.8</v>
+        <v>129.05</v>
       </c>
       <c r="D28" t="n">
-        <v>2.570694087403599</v>
+        <v>2.37325</v>
       </c>
       <c r="E28" t="n">
-        <v>0.3855889335432075</v>
+        <v>0.3409327435291203</v>
       </c>
       <c r="F28" t="n">
-        <v>2.593435425677081</v>
+        <v>2.933129829797607</v>
       </c>
       <c r="G28" t="n">
-        <v>0.7210241200271663</v>
+        <v>0.8226455813140677</v>
       </c>
       <c r="H28" t="n">
-        <v>0.008846380588384503</v>
+        <v>0.2359127061192909</v>
       </c>
       <c r="M28" t="n">
-        <v>4.788596911749426e-06</v>
+        <v>0.003603050848439052</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>288.15</v>
+        <v>661.5599999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>52.5</v>
+        <v>132.95</v>
       </c>
       <c r="D29" t="n">
-        <v>3.278688524590164</v>
+        <v>2.37075</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3001705699119376</v>
+        <v>0.3464298272680519</v>
       </c>
       <c r="F29" t="n">
-        <v>3.331439189036335</v>
+        <v>2.886587473965528</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6577708621912863</v>
+        <v>0.837336884929739</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01608895265608217</v>
+        <v>0.2175840868777929</v>
       </c>
       <c r="M29" t="n">
-        <v>2.57651166621531e-05</v>
+        <v>0.003058486201691223</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0,1770;0,8230</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>288.15</v>
+        <v>679.9299999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>69.5</v>
+        <v>136.84</v>
       </c>
       <c r="D30" t="n">
-        <v>5.917159763313609</v>
+        <v>2.36824</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1555582409719578</v>
+        <v>0.3514422905329327</v>
       </c>
       <c r="F30" t="n">
-        <v>6.428460451544115</v>
+        <v>2.845417375591264</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4512581371508471</v>
+        <v>0.8506849013983281</v>
       </c>
       <c r="H30" t="n">
-        <v>0.08640981631095548</v>
+        <v>0.2014902947299533</v>
       </c>
       <c r="M30" t="n">
-        <v>0.002420633275786934</v>
+        <v>0.002617221238806514</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0,1820;0,8180</t>
+          <t>0,1739;0,8261</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>288.15</v>
+        <v>698.45</v>
       </c>
       <c r="C31" t="n">
-        <v>81.90000000000001</v>
+        <v>140.74</v>
       </c>
       <c r="D31" t="n">
-        <v>10.94091903719912</v>
+        <v>2.36568</v>
       </c>
       <c r="E31" t="n">
-        <v>0.07523648459034767</v>
+        <v>0.3560633637396605</v>
       </c>
       <c r="F31" t="n">
-        <v>13.29142377458042</v>
+        <v>2.808488886633</v>
       </c>
       <c r="G31" t="n">
-        <v>0.257193278703954</v>
+        <v>0.8629295821443852</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2148361329966502</v>
+        <v>0.1871803822296337</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0511562270412213</v>
+        <v>0.00225378977104778</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0,1820;0,8180</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>288.15</v>
+        <v>501.13</v>
       </c>
       <c r="C32" t="n">
-        <v>96.59999999999999</v>
+        <v>107.18</v>
       </c>
       <c r="D32" t="n">
-        <v>13.58695652173913</v>
+        <v>2.68235</v>
       </c>
       <c r="E32" t="n">
-        <v>0.06512383667597073</v>
+        <v>0.2556597504877213</v>
       </c>
       <c r="F32" t="n">
-        <v>15.35536066426163</v>
+        <v>3.911448705133691</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2625816197447667</v>
+        <v>0.6576450460916737</v>
       </c>
       <c r="H32" t="n">
-        <v>0.1301545448896562</v>
+        <v>0.458217124958969</v>
       </c>
       <c r="M32" t="n">
-        <v>0.02895604825269211</v>
+        <v>0.017364179620245</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0,1820;0,8180</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>288.15</v>
+        <v>518.38</v>
       </c>
       <c r="C33" t="n">
-        <v>104.8</v>
+        <v>111.73</v>
       </c>
       <c r="D33" t="n">
-        <v>15.84786053882726</v>
+        <v>2.67989</v>
       </c>
       <c r="E33" t="n">
-        <v>0.06224245611990803</v>
+        <v>0.2676162371000017</v>
       </c>
       <c r="F33" t="n">
-        <v>16.06620404043075</v>
+        <v>3.736694046805256</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2722671357141015</v>
+        <v>0.6937449955662408</v>
       </c>
       <c r="H33" t="n">
-        <v>0.01377747495118024</v>
+        <v>0.3943460540564186</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0004414248582636421</v>
+        <v>0.01283718153268925</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0,1820;0,8180</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>288.15</v>
+        <v>535.97</v>
       </c>
       <c r="C34" t="n">
-        <v>124.1</v>
+        <v>116.32</v>
       </c>
       <c r="D34" t="n">
-        <v>17.18213058419244</v>
+        <v>2.67735</v>
       </c>
       <c r="E34" t="n">
-        <v>0.05782995279949796</v>
+        <v>0.2774233342998638</v>
       </c>
       <c r="F34" t="n">
-        <v>17.29207705679956</v>
+        <v>3.604599456364082</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2995517336590605</v>
+        <v>0.7241403392954737</v>
       </c>
       <c r="H34" t="n">
-        <v>0.006398884705734202</v>
+        <v>0.3463310573380702</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0001119280262846991</v>
+        <v>0.009882661543994094</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0,1820;0,8180</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>288.15</v>
+        <v>553.48</v>
       </c>
       <c r="C35" t="n">
-        <v>143.4</v>
+        <v>120.78</v>
       </c>
       <c r="D35" t="n">
-        <v>18.05054151624549</v>
+        <v>2.67481</v>
       </c>
       <c r="E35" t="n">
-        <v>0.05496934014864713</v>
+        <v>0.2857854136765619</v>
       </c>
       <c r="F35" t="n">
-        <v>18.19195932306659</v>
+        <v>3.499128899320774</v>
       </c>
       <c r="G35" t="n">
-        <v>0.3290159053063108</v>
+        <v>0.7500651610867178</v>
       </c>
       <c r="H35" t="n">
-        <v>0.007834546497889299</v>
+        <v>0.3081784871900338</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0001851758896860351</v>
+        <v>0.007810363767556467</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>288.15</v>
+        <v>571.42</v>
       </c>
       <c r="C36" t="n">
-        <v>25.8</v>
+        <v>125.32</v>
       </c>
       <c r="D36" t="n">
-        <v>1.251564455569462</v>
+        <v>2.67218</v>
       </c>
       <c r="E36" t="n">
-        <v>0.7995183252060329</v>
+        <v>0.2930876807575432</v>
       </c>
       <c r="F36" t="n">
-        <v>1.250753070284291</v>
+        <v>3.411948251851808</v>
       </c>
       <c r="G36" t="n">
-        <v>0.8609845264329931</v>
+        <v>0.7730869738078228</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0006482968428514482</v>
+        <v>0.2768407262429206</v>
       </c>
       <c r="M36" t="n">
-        <v>6.095797046219054e-09</v>
+        <v>0.006290311108596315</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>288.15</v>
+        <v>589.27</v>
       </c>
       <c r="C37" t="n">
-        <v>29.6</v>
+        <v>129.78</v>
       </c>
       <c r="D37" t="n">
-        <v>1.470588235294118</v>
+        <v>2.66954</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6788341644633499</v>
+        <v>0.2994761586334022</v>
       </c>
       <c r="F37" t="n">
-        <v>1.47311383596986</v>
+        <v>3.339163974064895</v>
       </c>
       <c r="G37" t="n">
-        <v>0.8386922319811567</v>
+        <v>0.7932709200906787</v>
       </c>
       <c r="H37" t="n">
-        <v>0.001717408459504659</v>
+        <v>0.2508387115626267</v>
       </c>
       <c r="M37" t="n">
-        <v>5.906165530841836e-08</v>
+        <v>0.005153980076350145</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>288.15</v>
+        <v>607.24</v>
       </c>
       <c r="C38" t="n">
-        <v>33.4</v>
+        <v>134.39</v>
       </c>
       <c r="D38" t="n">
-        <v>1.703577512776831</v>
+        <v>2.66685</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5851673336533545</v>
+        <v>0.3047293498344559</v>
       </c>
       <c r="F38" t="n">
-        <v>1.708912891218201</v>
+        <v>3.281600543378082</v>
       </c>
       <c r="G38" t="n">
-        <v>0.8157813247032458</v>
+        <v>0.8111229870907133</v>
       </c>
       <c r="H38" t="n">
-        <v>0.003131867145084254</v>
+        <v>0.2305156058188807</v>
       </c>
       <c r="M38" t="n">
-        <v>2.635765103021938e-07</v>
+        <v>0.004343887707858013</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>288.15</v>
+        <v>625.4299999999999</v>
       </c>
       <c r="C39" t="n">
-        <v>41</v>
+        <v>138.88</v>
       </c>
       <c r="D39" t="n">
-        <v>2.212389380530973</v>
+        <v>2.66412</v>
       </c>
       <c r="E39" t="n">
-        <v>0.4486482004773343</v>
+        <v>0.3098540059436929</v>
       </c>
       <c r="F39" t="n">
-        <v>2.228917889197061</v>
+        <v>3.227326356341255</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7677803712697665</v>
+        <v>0.8275303981267673</v>
       </c>
       <c r="H39" t="n">
-        <v>0.007470885917071783</v>
+        <v>0.2114042747103191</v>
       </c>
       <c r="M39" t="n">
-        <v>2.529551840045802e-06</v>
+        <v>0.003645993101416012</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>288.15</v>
+        <v>643.7</v>
       </c>
       <c r="C40" t="n">
-        <v>48.7</v>
+        <v>143.35</v>
       </c>
       <c r="D40" t="n">
-        <v>2.793296089385475</v>
+        <v>2.66135</v>
       </c>
       <c r="E40" t="n">
-        <v>0.3519565234706467</v>
+        <v>0.3145133289159808</v>
       </c>
       <c r="F40" t="n">
-        <v>2.841260023081801</v>
+        <v>3.179515486503087</v>
       </c>
       <c r="G40" t="n">
-        <v>0.7154267895399851</v>
+        <v>0.8424014108011161</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01717108826328479</v>
+        <v>0.1947002410442394</v>
       </c>
       <c r="M40" t="n">
-        <v>2.130128644097758e-05</v>
+        <v>0.003086154843712417</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>288.15</v>
+        <v>662.14</v>
       </c>
       <c r="C41" t="n">
-        <v>56.4</v>
+        <v>147.85</v>
       </c>
       <c r="D41" t="n">
-        <v>3.484320557491289</v>
+        <v>2.65853</v>
       </c>
       <c r="E41" t="n">
-        <v>0.2794797012887106</v>
+        <v>0.3187365677849847</v>
       </c>
       <c r="F41" t="n">
-        <v>3.57807738948086</v>
+        <v>3.1373871123397</v>
       </c>
       <c r="G41" t="n">
-        <v>0.6579253080290265</v>
+        <v>0.8559910781919572</v>
       </c>
       <c r="H41" t="n">
-        <v>0.02690821078100661</v>
+        <v>0.1801210113633095</v>
       </c>
       <c r="M41" t="n">
-        <v>8.139206985852288e-05</v>
+        <v>0.002635679701589833</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>288.15</v>
+        <v>680.42</v>
       </c>
       <c r="C42" t="n">
-        <v>66.5</v>
+        <v>152.28</v>
       </c>
       <c r="D42" t="n">
-        <v>4.62962962962963</v>
+        <v>2.65572</v>
       </c>
       <c r="E42" t="n">
-        <v>0.205452349665825</v>
+        <v>0.3225692468884551</v>
       </c>
       <c r="F42" t="n">
-        <v>4.867308656369872</v>
+        <v>3.100109541272548</v>
       </c>
       <c r="G42" t="n">
-        <v>0.5702692783756651</v>
+        <v>0.868269608173327</v>
       </c>
       <c r="H42" t="n">
-        <v>0.05133866977589227</v>
+        <v>0.1673329798595292</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0005230677754832284</v>
+        <v>0.002269908786119842</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,2634;0,7366</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>288.15</v>
+        <v>698.6</v>
       </c>
       <c r="C43" t="n">
-        <v>74.2</v>
+        <v>156.65</v>
       </c>
       <c r="D43" t="n">
-        <v>5.847953216374268</v>
+        <v>2.65291</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1572224251142389</v>
+        <v>0.3260974608923473</v>
       </c>
       <c r="F43" t="n">
-        <v>6.360415820283863</v>
+        <v>3.066567882079046</v>
       </c>
       <c r="G43" t="n">
-        <v>0.4869289704750195</v>
+        <v>0.8794579460259641</v>
       </c>
       <c r="H43" t="n">
-        <v>0.08763110526854068</v>
+        <v>0.1559260894938186</v>
       </c>
       <c r="M43" t="n">
-        <v>0.002431647411164833</v>
+        <v>0.001966814292024394</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>288.15</v>
+        <v>518.58</v>
       </c>
       <c r="C44" t="n">
-        <v>89.59999999999999</v>
+        <v>120.88</v>
       </c>
       <c r="D44" t="n">
-        <v>9.615384615384615</v>
+        <v>2.98057</v>
       </c>
       <c r="E44" t="n">
-        <v>0.08625946136667877</v>
+        <v>0.2599919648537726</v>
       </c>
       <c r="F44" t="n">
-        <v>11.59293118872048</v>
+        <v>3.846272712937226</v>
       </c>
       <c r="G44" t="n">
-        <v>0.3225982221761952</v>
+        <v>0.7288941356349775</v>
       </c>
       <c r="H44" t="n">
-        <v>0.2056648436269305</v>
+        <v>0.2904487104604911</v>
       </c>
       <c r="M44" t="n">
-        <v>0.03621009675659667</v>
+        <v>0.008614266519389345</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>288.15</v>
+        <v>536.1</v>
       </c>
       <c r="C45" t="n">
-        <v>104.8</v>
+        <v>126.21</v>
       </c>
       <c r="D45" t="n">
-        <v>13.22751322751323</v>
+        <v>2.97776</v>
       </c>
       <c r="E45" t="n">
-        <v>0.07073984448727701</v>
+        <v>0.2663399048121171</v>
       </c>
       <c r="F45" t="n">
-        <v>14.13630475509253</v>
+        <v>3.75460072611134</v>
       </c>
       <c r="G45" t="n">
-        <v>0.3094372561762003</v>
+        <v>0.7541366400937455</v>
       </c>
       <c r="H45" t="n">
-        <v>0.06870463948499522</v>
+        <v>0.2608809058189174</v>
       </c>
       <c r="M45" t="n">
-        <v>0.007647241116665936</v>
+        <v>0.006936569123507967</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>288.15</v>
+        <v>553.6</v>
       </c>
       <c r="C46" t="n">
-        <v>124.1</v>
+        <v>131.43</v>
       </c>
       <c r="D46" t="n">
-        <v>15.625</v>
+        <v>2.97493</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0631571179661759</v>
+        <v>0.2718950391354112</v>
       </c>
       <c r="F46" t="n">
-        <v>15.83352806781897</v>
+        <v>3.677889832708468</v>
       </c>
       <c r="G46" t="n">
-        <v>0.327145765539031</v>
+        <v>0.7763642918105141</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01334579634041415</v>
+        <v>0.2362945792702579</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0004026292135954947</v>
+        <v>0.00567991409656917</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>0,2470;0,7530</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>288.15</v>
+        <v>571.46</v>
       </c>
       <c r="C47" t="n">
-        <v>143.3</v>
+        <v>136.65</v>
       </c>
       <c r="D47" t="n">
-        <v>16.97792869269949</v>
+        <v>2.97202</v>
       </c>
       <c r="E47" t="n">
-        <v>0.05893356311669794</v>
+        <v>0.2769727021549116</v>
       </c>
       <c r="F47" t="n">
-        <v>16.96825963194927</v>
+        <v>3.61046410790583</v>
       </c>
       <c r="G47" t="n">
-        <v>0.3524975540181641</v>
+        <v>0.7965748843950208</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0005695076781879387</v>
+        <v>0.2148182407607721</v>
       </c>
       <c r="M47" t="n">
-        <v>8.656549610318388e-07</v>
+        <v>0.004685182516318056</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>288.15</v>
+        <v>589.38</v>
       </c>
       <c r="C48" t="n">
-        <v>26.2</v>
+        <v>141.84</v>
       </c>
       <c r="D48" t="n">
-        <v>1.262626262626263</v>
+        <v>2.96906</v>
       </c>
       <c r="E48" t="n">
-        <v>0.7914186824900127</v>
+        <v>0.2814676207062664</v>
       </c>
       <c r="F48" t="n">
-        <v>1.263553694302155</v>
+        <v>3.552806527055482</v>
       </c>
       <c r="G48" t="n">
-        <v>0.8654755582631323</v>
+        <v>0.8146998045688513</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0007345258873070258</v>
+        <v>0.1966098789029127</v>
       </c>
       <c r="M48" t="n">
-        <v>7.96416216156629e-09</v>
+        <v>0.003916781699417662</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>288.15</v>
+        <v>607.34</v>
       </c>
       <c r="C49" t="n">
-        <v>33.4</v>
+        <v>146.98</v>
       </c>
       <c r="D49" t="n">
-        <v>1.683501683501684</v>
+        <v>2.96608</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5919590610360533</v>
+        <v>0.285527878300587</v>
       </c>
       <c r="F49" t="n">
-        <v>1.689306010874787</v>
+        <v>3.502284981599096</v>
       </c>
       <c r="G49" t="n">
-        <v>0.8252496665648638</v>
+        <v>0.831075956518908</v>
       </c>
       <c r="H49" t="n">
-        <v>0.003447770459623572</v>
+        <v>0.1807790017798225</v>
       </c>
       <c r="M49" t="n">
-        <v>3.119464467977815e-07</v>
+        <v>0.003304779106800998</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>288.15</v>
+        <v>625.47</v>
       </c>
       <c r="C50" t="n">
-        <v>41.1</v>
+        <v>152.19</v>
       </c>
       <c r="D50" t="n">
-        <v>2.173913043478261</v>
+        <v>2.96304</v>
       </c>
       <c r="E50" t="n">
-        <v>0.4547386994587934</v>
+        <v>0.2890798825529917</v>
       </c>
       <c r="F50" t="n">
-        <v>2.199065092085078</v>
+        <v>3.459251440012221</v>
       </c>
       <c r="G50" t="n">
-        <v>0.7801012168484924</v>
+        <v>0.8459863282470607</v>
       </c>
       <c r="H50" t="n">
-        <v>0.01156994235913586</v>
+        <v>0.167467006861946</v>
       </c>
       <c r="M50" t="n">
-        <v>5.857643973330454e-06</v>
+        <v>0.002830181531023007</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>288.15</v>
+        <v>643.6799999999999</v>
       </c>
       <c r="C51" t="n">
-        <v>48.7</v>
+        <v>157.28</v>
       </c>
       <c r="D51" t="n">
-        <v>2.73224043715847</v>
+        <v>2.95997</v>
       </c>
       <c r="E51" t="n">
-        <v>0.3605412804312952</v>
+        <v>0.2925352234934358</v>
       </c>
       <c r="F51" t="n">
-        <v>2.773607501487088</v>
+        <v>3.418391768546939</v>
       </c>
       <c r="G51" t="n">
-        <v>0.7328771412219878</v>
+        <v>0.859701121387317</v>
       </c>
       <c r="H51" t="n">
-        <v>0.01514034554427408</v>
+        <v>0.1548737887704737</v>
       </c>
       <c r="M51" t="n">
-        <v>1.584475936266662e-05</v>
+        <v>0.002415523193996589</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>288.15</v>
+        <v>662.0700000000001</v>
       </c>
       <c r="C52" t="n">
-        <v>56.4</v>
+        <v>162.39</v>
       </c>
       <c r="D52" t="n">
-        <v>3.367003367003367</v>
+        <v>2.95684</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2895375193627656</v>
+        <v>0.2957080855475066</v>
       </c>
       <c r="F52" t="n">
-        <v>3.453783821180999</v>
+        <v>3.381713415608807</v>
       </c>
       <c r="G52" t="n">
-        <v>0.6816024946868035</v>
+        <v>0.8723372423357357</v>
       </c>
       <c r="H52" t="n">
-        <v>0.02577379489075671</v>
+        <v>0.1436917167005341</v>
       </c>
       <c r="M52" t="n">
-        <v>6.973006691922308e-05</v>
+        <v>0.002074912865414876</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>288.15</v>
+        <v>680.33</v>
       </c>
       <c r="C53" t="n">
-        <v>66.5</v>
+        <v>167.42</v>
       </c>
       <c r="D53" t="n">
-        <v>4.385964912280701</v>
+        <v>2.95372</v>
       </c>
       <c r="E53" t="n">
-        <v>0.2187885764269223</v>
+        <v>0.2986203598134207</v>
       </c>
       <c r="F53" t="n">
-        <v>4.570622544975562</v>
+        <v>3.3487334909944</v>
       </c>
       <c r="G53" t="n">
-        <v>0.6072863308633848</v>
+        <v>0.8838386147173353</v>
       </c>
       <c r="H53" t="n">
-        <v>0.04210194025442822</v>
+        <v>0.1337342371634415</v>
       </c>
       <c r="M53" t="n">
-        <v>0.0003157263084487967</v>
+        <v>0.001793513311121646</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,3377;0,6623</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>288.15</v>
+        <v>698.6</v>
       </c>
       <c r="C54" t="n">
-        <v>74.2</v>
+        <v>172.41</v>
       </c>
       <c r="D54" t="n">
-        <v>5.319148936170213</v>
+        <v>2.95057</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1754391117244043</v>
+        <v>0.3013316695733775</v>
       </c>
       <c r="F54" t="n">
-        <v>5.699983260123267</v>
+        <v>3.318602393886412</v>
       </c>
       <c r="G54" t="n">
-        <v>0.5433473373212804</v>
+        <v>0.8944261549192627</v>
       </c>
       <c r="H54" t="n">
-        <v>0.07159685290317412</v>
+        <v>0.1247326428067837</v>
       </c>
       <c r="M54" t="n">
-        <v>0.001342914650933144</v>
+        <v>0.001556871758043253</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>288.15</v>
+        <v>554.25</v>
       </c>
       <c r="C55" t="n">
-        <v>89.59999999999999</v>
+        <v>141.81</v>
       </c>
       <c r="D55" t="n">
-        <v>8</v>
+        <v>3.28877</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1085311916438681</v>
+        <v>0.2598793736978174</v>
       </c>
       <c r="F55" t="n">
-        <v>9.213941032559365</v>
+        <v>3.847939087165803</v>
       </c>
       <c r="G55" t="n">
-        <v>0.4058913529049761</v>
+        <v>0.7997215677487912</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1517426290699206</v>
+        <v>0.1700237739841347</v>
       </c>
       <c r="M55" t="n">
-        <v>0.01364493361603053</v>
+        <v>0.003593908828067094</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>288.15</v>
+        <v>571.52</v>
       </c>
       <c r="C56" t="n">
-        <v>104.8</v>
+        <v>147.65</v>
       </c>
       <c r="D56" t="n">
-        <v>11.16071428571429</v>
+        <v>3.28565</v>
       </c>
       <c r="E56" t="n">
-        <v>0.08067369077384719</v>
+        <v>0.2630069248149758</v>
       </c>
       <c r="F56" t="n">
-        <v>12.39561485792565</v>
+        <v>3.80218125702772</v>
       </c>
       <c r="G56" t="n">
-        <v>0.3528908735890188</v>
+        <v>0.8172125806284296</v>
       </c>
       <c r="H56" t="n">
-        <v>0.1106470912701385</v>
+        <v>0.1572082409957605</v>
       </c>
       <c r="M56" t="n">
-        <v>0.01412017984488855</v>
+        <v>0.003066718844673989</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0,3000;0,7000</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>288.15</v>
+        <v>589.36</v>
       </c>
       <c r="C57" t="n">
-        <v>143.3</v>
+        <v>153.59</v>
       </c>
       <c r="D57" t="n">
-        <v>15.625</v>
+        <v>3.2824</v>
       </c>
       <c r="E57" t="n">
-        <v>0.06281367843296579</v>
+        <v>0.2659699514324753</v>
       </c>
       <c r="F57" t="n">
-        <v>15.92009933102694</v>
+        <v>3.759823222939833</v>
       </c>
       <c r="G57" t="n">
-        <v>0.3757055714187836</v>
+        <v>0.8336441358448177</v>
       </c>
       <c r="H57" t="n">
-        <v>0.01888635718572425</v>
+        <v>0.1454494342370927</v>
       </c>
       <c r="M57" t="n">
-        <v>0.0008063297701161884</v>
+        <v>0.002619918779336295</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0,2140;0,7860</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>273.15</v>
+        <v>607.24</v>
       </c>
       <c r="C58" t="n">
-        <v>23.9</v>
+        <v>159.46</v>
       </c>
       <c r="D58" t="n">
-        <v>1.262626262626263</v>
+        <v>3.27911</v>
       </c>
       <c r="E58" t="n">
-        <v>0.7992613768567023</v>
+        <v>0.2687047539991694</v>
       </c>
       <c r="F58" t="n">
-        <v>1.251155165201093</v>
+        <v>3.721556783483969</v>
       </c>
       <c r="G58" t="n">
-        <v>0.8411072277177795</v>
+        <v>0.8486577475415681</v>
       </c>
       <c r="H58" t="n">
-        <v>0.009085109160734593</v>
+        <v>0.1349289238494497</v>
       </c>
       <c r="M58" t="n">
-        <v>1.218389593867967e-06</v>
+        <v>0.002250105243854141</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0,2140;0,7860</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>273.15</v>
+        <v>625.26</v>
       </c>
       <c r="C59" t="n">
-        <v>29.4</v>
+        <v>165.4</v>
       </c>
       <c r="D59" t="n">
-        <v>1.623376623376623</v>
+        <v>3.27577</v>
       </c>
       <c r="E59" t="n">
-        <v>0.6172886577922202</v>
+        <v>0.2710707899478588</v>
       </c>
       <c r="F59" t="n">
-        <v>1.6199876465843</v>
+        <v>3.689073249804424</v>
       </c>
       <c r="G59" t="n">
-        <v>0.7990984067632552</v>
+        <v>0.8624291403371973</v>
       </c>
       <c r="H59" t="n">
-        <v>0.002087609704071362</v>
+        <v>0.1261698012389222</v>
       </c>
       <c r="M59" t="n">
-        <v>1.063441083232243e-07</v>
+        <v>0.001963443405734463</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0,2140;0,7860</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>273.15</v>
+        <v>643.5700000000001</v>
       </c>
       <c r="C60" t="n">
-        <v>33.2</v>
+        <v>171.24</v>
       </c>
       <c r="D60" t="n">
-        <v>1.901140684410646</v>
+        <v>3.27235</v>
       </c>
       <c r="E60" t="n">
-        <v>0.5255120752115743</v>
+        <v>0.2735295981756214</v>
       </c>
       <c r="F60" t="n">
-        <v>1.902905845878792</v>
+        <v>3.65591148698264</v>
       </c>
       <c r="G60" t="n">
-        <v>0.7682196657837913</v>
+        <v>0.8753456893063014</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0009284749322445528</v>
+        <v>0.1172128552821796</v>
       </c>
       <c r="M60" t="n">
-        <v>2.884995378357138e-08</v>
+        <v>0.001691027750532576</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0,2140;0,7860</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>273.15</v>
+        <v>661.99</v>
       </c>
       <c r="C61" t="n">
-        <v>40.9</v>
+        <v>177.07</v>
       </c>
       <c r="D61" t="n">
-        <v>2.544529262086514</v>
+        <v>3.26889</v>
       </c>
       <c r="E61" t="n">
-        <v>0.388235730995157</v>
+        <v>0.2758013088092185</v>
       </c>
       <c r="F61" t="n">
-        <v>2.575754677285163</v>
+        <v>3.625798602325471</v>
       </c>
       <c r="G61" t="n">
-        <v>0.6991710669113879</v>
+        <v>0.8872698476604978</v>
       </c>
       <c r="H61" t="n">
-        <v>0.012271588173069</v>
+        <v>0.1091834238305575</v>
       </c>
       <c r="M61" t="n">
-        <v>9.028023651185286e-06</v>
+        <v>0.001464181039240474</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>0,2140;0,7860</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>273.15</v>
+        <v>680.3200000000001</v>
       </c>
       <c r="C62" t="n">
-        <v>44.7</v>
+        <v>182.8</v>
       </c>
       <c r="D62" t="n">
-        <v>2.923976608187134</v>
+        <v>3.26541</v>
       </c>
       <c r="E62" t="n">
-        <v>0.335566897475274</v>
+        <v>0.2779372504510718</v>
       </c>
       <c r="F62" t="n">
-        <v>2.980031723998295</v>
+        <v>3.597934420006938</v>
       </c>
       <c r="G62" t="n">
-        <v>0.6604672277636296</v>
+        <v>0.8982051725851621</v>
       </c>
       <c r="H62" t="n">
-        <v>0.01917084960741717</v>
+        <v>0.1018323640850424</v>
       </c>
       <c r="M62" t="n">
-        <v>2.90942223018769e-05</v>
+        <v>0.001270948159781043</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4009;0,5991</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>273.15</v>
+        <v>698.53</v>
       </c>
       <c r="C63" t="n">
-        <v>24</v>
+        <v>188.45</v>
       </c>
       <c r="D63" t="n">
-        <v>1.228501228501229</v>
+        <v>3.26194</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8070468717200074</v>
+        <v>0.2799124431418916</v>
       </c>
       <c r="F63" t="n">
-        <v>1.239085405124939</v>
+        <v>3.572545717423093</v>
       </c>
       <c r="G63" t="n">
-        <v>0.8528538951406959</v>
+        <v>0.9082368655443048</v>
       </c>
       <c r="H63" t="n">
-        <v>0.008615519771700143</v>
+        <v>0.09522116207627766</v>
       </c>
       <c r="M63" t="n">
-        <v>1.037266618536061e-06</v>
+        <v>0.001108918525240395</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>273.15</v>
+        <v>571.65</v>
       </c>
       <c r="C64" t="n">
-        <v>33.2</v>
+        <v>158.38</v>
       </c>
       <c r="D64" t="n">
-        <v>1.824817518248175</v>
+        <v>3.62692</v>
       </c>
       <c r="E64" t="n">
-        <v>0.5393930612098812</v>
+        <v>0.2510892549643206</v>
       </c>
       <c r="F64" t="n">
-        <v>1.853935602651169</v>
+        <v>3.982647525646204</v>
       </c>
       <c r="G64" t="n">
-        <v>0.7885115809031072</v>
+        <v>0.8366890799954591</v>
       </c>
       <c r="H64" t="n">
-        <v>0.01595671025284078</v>
+        <v>0.09807978274850378</v>
       </c>
       <c r="M64" t="n">
-        <v>7.85058184536935e-06</v>
+        <v>0.001454506580487015</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>273.15</v>
+        <v>589.67</v>
       </c>
       <c r="C65" t="n">
-        <v>40.9</v>
+        <v>165.34</v>
       </c>
       <c r="D65" t="n">
-        <v>1.934235976789168</v>
+        <v>3.62329</v>
       </c>
       <c r="E65" t="n">
-        <v>0.404860568184143</v>
+        <v>0.2525995975720458</v>
       </c>
       <c r="F65" t="n">
-        <v>2.469986159642915</v>
+        <v>3.95883449384666</v>
       </c>
       <c r="G65" t="n">
-        <v>0.7291106222553974</v>
+        <v>0.8518583728513168</v>
       </c>
       <c r="H65" t="n">
-        <v>0.2769828445353873</v>
+        <v>0.09260768358223054</v>
       </c>
       <c r="M65" t="n">
-        <v>0.002657669059516885</v>
+        <v>0.001294139164951854</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>273.15</v>
+        <v>607.48</v>
       </c>
       <c r="C66" t="n">
-        <v>48.6</v>
+        <v>172.08</v>
       </c>
       <c r="D66" t="n">
-        <v>3.08641975308642</v>
+        <v>3.61967</v>
       </c>
       <c r="E66" t="n">
-        <v>0.3093303655100909</v>
+        <v>0.2540961543968968</v>
       </c>
       <c r="F66" t="n">
-        <v>3.232789636901581</v>
+        <v>3.935518041874832</v>
       </c>
       <c r="G66" t="n">
-        <v>0.6619473702442615</v>
+        <v>0.8656898935571751</v>
       </c>
       <c r="H66" t="n">
-        <v>0.04742384235611218</v>
+        <v>0.087258794827935</v>
       </c>
       <c r="M66" t="n">
-        <v>0.0001983716934079976</v>
+        <v>0.001146666500645578</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>273.15</v>
+        <v>625.58</v>
       </c>
       <c r="C67" t="n">
-        <v>56.2</v>
+        <v>178.87</v>
       </c>
       <c r="D67" t="n">
-        <v>3.952569169960474</v>
+        <v>3.61596</v>
       </c>
       <c r="E67" t="n">
-        <v>0.235318283540609</v>
+        <v>0.2554992961172481</v>
       </c>
       <c r="F67" t="n">
-        <v>4.249563548373535</v>
+        <v>3.913905107359286</v>
       </c>
       <c r="G67" t="n">
-        <v>0.5823131862098476</v>
+        <v>0.8786384435662884</v>
       </c>
       <c r="H67" t="n">
-        <v>0.07513957773850446</v>
+        <v>0.08239723541169865</v>
       </c>
       <c r="M67" t="n">
-        <v>0.0008167190815644494</v>
+        <v>0.001020359620682027</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0,3010;0,6990</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>273.15</v>
+        <v>643.87</v>
       </c>
       <c r="C68" t="n">
-        <v>60.1</v>
+        <v>185.61</v>
       </c>
       <c r="D68" t="n">
-        <v>4.484304932735426</v>
+        <v>3.61218</v>
       </c>
       <c r="E68" t="n">
-        <v>0.2008297882832348</v>
+        <v>0.2569099200033585</v>
       </c>
       <c r="F68" t="n">
-        <v>4.97934100587547</v>
+        <v>3.892414897746757</v>
       </c>
       <c r="G68" t="n">
-        <v>0.531455908329063</v>
+        <v>0.8907378277497</v>
       </c>
       <c r="H68" t="n">
-        <v>0.1103930443102298</v>
+        <v>0.07758054630354982</v>
       </c>
       <c r="M68" t="n">
-        <v>0.002269080682499214</v>
+        <v>0.0009026620450015531</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>273.15</v>
+        <v>662.09</v>
       </c>
       <c r="C69" t="n">
-        <v>85.59999999999999</v>
+        <v>192.19</v>
       </c>
       <c r="D69" t="n">
-        <v>11.1731843575419</v>
+        <v>3.60839</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0685980902699606</v>
+        <v>0.2583335243136912</v>
       </c>
       <c r="F69" t="n">
-        <v>14.57766529745369</v>
+        <v>3.870964880213194</v>
       </c>
       <c r="G69" t="n">
-        <v>0.2585535036172525</v>
+        <v>0.9019041164927423</v>
       </c>
       <c r="H69" t="n">
-        <v>0.304701044122105</v>
+        <v>0.07276787714553976</v>
       </c>
       <c r="M69" t="n">
-        <v>0.1073193562057652</v>
+        <v>0.0007924777898732561</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>273.15</v>
+        <v>680.42</v>
       </c>
       <c r="C70" t="n">
-        <v>89.5</v>
+        <v>198.74</v>
       </c>
       <c r="D70" t="n">
-        <v>12.18026796589525</v>
+        <v>3.60455</v>
       </c>
       <c r="E70" t="n">
-        <v>0.06640617030822789</v>
+        <v>0.2596967058236997</v>
       </c>
       <c r="F70" t="n">
-        <v>15.05884160099047</v>
+        <v>3.850645686198538</v>
       </c>
       <c r="G70" t="n">
-        <v>0.2616954111702833</v>
+        <v>0.9123059296828586</v>
       </c>
       <c r="H70" t="n">
-        <v>0.2363308954413171</v>
+        <v>0.06827362255996947</v>
       </c>
       <c r="M70" t="n">
-        <v>0.07672394604319704</v>
+        <v>0.0006961274340865432</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,4573;0,5427</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>273.15</v>
+        <v>698.66</v>
       </c>
       <c r="C71" t="n">
-        <v>97.2</v>
+        <v>205.17</v>
       </c>
       <c r="D71" t="n">
-        <v>13.67989056087551</v>
+        <v>3.60071</v>
       </c>
       <c r="E71" t="n">
-        <v>0.06320550986651076</v>
+        <v>0.2610215422442308</v>
       </c>
       <c r="F71" t="n">
-        <v>15.82140547733872</v>
+        <v>3.83110141562311</v>
       </c>
       <c r="G71" t="n">
-        <v>0.2705115676056683</v>
+        <v>0.9219134950888203</v>
       </c>
       <c r="H71" t="n">
-        <v>0.1565447403934605</v>
+        <v>0.06398499618772692</v>
       </c>
       <c r="M71" t="n">
-        <v>0.0424637605318002</v>
+        <v>0.0006101172918715022</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>273.15</v>
+        <v>607.66</v>
       </c>
       <c r="C72" t="n">
-        <v>104.7</v>
+        <v>193.16</v>
       </c>
       <c r="D72" t="n">
-        <v>14.64128843338214</v>
+        <v>4.26175</v>
       </c>
       <c r="E72" t="n">
-        <v>0.06091606963463075</v>
+        <v>0.2333974480925638</v>
       </c>
       <c r="F72" t="n">
-        <v>16.41602956326487</v>
+        <v>4.2845369911817</v>
       </c>
       <c r="G72" t="n">
-        <v>0.2808298016924337</v>
+        <v>0.8923156144949762</v>
       </c>
       <c r="H72" t="n">
-        <v>0.1212148191709906</v>
+        <v>0.005346862481773768</v>
       </c>
       <c r="M72" t="n">
-        <v>0.02916394516756888</v>
+        <v>5.968355943848785e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>273.15</v>
+        <v>625.8</v>
       </c>
       <c r="C73" t="n">
-        <v>120.1</v>
+        <v>201.75</v>
       </c>
       <c r="D73" t="n">
-        <v>15.94896331738437</v>
+        <v>4.257359999999999</v>
       </c>
       <c r="E73" t="n">
-        <v>0.05755209535128948</v>
+        <v>0.2331776236713343</v>
       </c>
       <c r="F73" t="n">
-        <v>17.37556198251598</v>
+        <v>4.288576168910221</v>
       </c>
       <c r="G73" t="n">
-        <v>0.3043468313664262</v>
+        <v>0.904129622794653</v>
       </c>
       <c r="H73" t="n">
-        <v>0.08944773630375176</v>
+        <v>0.007332283130912468</v>
       </c>
       <c r="M73" t="n">
-        <v>0.0188442939940304</v>
+        <v>1.120056553369516e-05</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>273.15</v>
+        <v>643.98</v>
       </c>
       <c r="C74" t="n">
-        <v>131.7</v>
+        <v>210.24</v>
       </c>
       <c r="D74" t="n">
-        <v>16.55629139072848</v>
+        <v>4.25293</v>
       </c>
       <c r="E74" t="n">
-        <v>0.05569571599270587</v>
+        <v>0.2330790041035828</v>
       </c>
       <c r="F74" t="n">
-        <v>17.95470229938267</v>
+        <v>4.290390736162531</v>
       </c>
       <c r="G74" t="n">
-        <v>0.3229774515934233</v>
+        <v>0.9151914705614164</v>
       </c>
       <c r="H74" t="n">
-        <v>0.08446401888271297</v>
+        <v>0.008808218372400017</v>
       </c>
       <c r="M74" t="n">
-        <v>0.01810697286521327</v>
+        <v>1.612996268780199e-05</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0,3210;0,6790</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>273.15</v>
+        <v>662.15</v>
       </c>
       <c r="C75" t="n">
-        <v>143.2</v>
+        <v>218.49</v>
       </c>
       <c r="D75" t="n">
-        <v>17.15265866209263</v>
+        <v>4.24847</v>
       </c>
       <c r="E75" t="n">
-        <v>0.05420211230844465</v>
+        <v>0.2332145916380212</v>
       </c>
       <c r="F75" t="n">
-        <v>18.44946548041082</v>
+        <v>4.287896366073558</v>
       </c>
       <c r="G75" t="n">
-        <v>0.3417620742414367</v>
+        <v>0.9255433034284845</v>
       </c>
       <c r="H75" t="n">
-        <v>0.07560383750795079</v>
+        <v>0.009280132865139184</v>
       </c>
       <c r="M75" t="n">
-        <v>0.0155713696670052</v>
+        <v>1.786710737662293e-05</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>273.15</v>
+        <v>680.48</v>
       </c>
       <c r="C76" t="n">
-        <v>85.59999999999999</v>
+        <v>226.67</v>
       </c>
       <c r="D76" t="n">
-        <v>10.34126163391934</v>
+        <v>4.243939999999999</v>
       </c>
       <c r="E76" t="n">
-        <v>0.07261537146663632</v>
+        <v>0.2334564667471344</v>
       </c>
       <c r="F76" t="n">
-        <v>13.77118893428036</v>
+        <v>4.283453844451171</v>
       </c>
       <c r="G76" t="n">
-        <v>0.273695064035751</v>
+        <v>0.9352989130869297</v>
       </c>
       <c r="H76" t="n">
-        <v>0.3316739699449109</v>
+        <v>0.00931065105801957</v>
       </c>
       <c r="M76" t="n">
-        <v>0.108929641534832</v>
+        <v>1.794648164725726e-05</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,5391;0,4609</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>273.15</v>
+        <v>698.75</v>
       </c>
       <c r="C77" t="n">
-        <v>89.5</v>
+        <v>234.69</v>
       </c>
       <c r="D77" t="n">
-        <v>11.38952164009112</v>
+        <v>4.2394</v>
       </c>
       <c r="E77" t="n">
-        <v>0.06968313503491473</v>
+        <v>0.2337813331327638</v>
       </c>
       <c r="F77" t="n">
-        <v>14.35067465748994</v>
+        <v>4.277501486537005</v>
       </c>
       <c r="G77" t="n">
-        <v>0.2746093712369516</v>
+        <v>0.9443836007422579</v>
       </c>
       <c r="H77" t="n">
-        <v>0.2599892349276165</v>
+        <v>0.008987471466954172</v>
       </c>
       <c r="M77" t="n">
-        <v>0.08118914067083469</v>
+        <v>1.668647444057026e-05</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,6007;0,3993</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>273.15</v>
+        <v>625.21</v>
       </c>
       <c r="C78" t="n">
-        <v>97.2</v>
+        <v>221.33</v>
       </c>
       <c r="D78" t="n">
-        <v>12.95336787564767</v>
+        <v>4.9144</v>
       </c>
       <c r="E78" t="n">
-        <v>0.06564394133218733</v>
+        <v>0.2172641422811517</v>
       </c>
       <c r="F78" t="n">
-        <v>15.23369833842789</v>
+        <v>4.60269232419377</v>
       </c>
       <c r="G78" t="n">
-        <v>0.2809477450793137</v>
+        <v>0.9250565138871394</v>
       </c>
       <c r="H78" t="n">
-        <v>0.176041511726633</v>
+        <v>0.06342741246260578</v>
       </c>
       <c r="M78" t="n">
-        <v>0.04814728721743939</v>
+        <v>0.001116800863868065</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,6007;0,3993</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>273.15</v>
+        <v>643.47</v>
       </c>
       <c r="C79" t="n">
-        <v>104.7</v>
+        <v>231.79</v>
       </c>
       <c r="D79" t="n">
-        <v>14.10437235543018</v>
+        <v>4.90925</v>
       </c>
       <c r="E79" t="n">
-        <v>0.06288854321678081</v>
+        <v>0.2159635386735347</v>
       </c>
       <c r="F79" t="n">
-        <v>15.90114747217051</v>
+        <v>4.630411254335244</v>
       </c>
       <c r="G79" t="n">
-        <v>0.2899231225229006</v>
+        <v>0.9356483768942438</v>
       </c>
       <c r="H79" t="n">
-        <v>0.1273913557768893</v>
+        <v>0.05679864453119236</v>
       </c>
       <c r="M79" t="n">
-        <v>0.02989260018645573</v>
+        <v>0.000893690184872351</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,6007;0,3993</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>273.15</v>
+        <v>661.66</v>
       </c>
       <c r="C80" t="n">
-        <v>120.1</v>
+        <v>242</v>
       </c>
       <c r="D80" t="n">
-        <v>15.47987616099071</v>
+        <v>4.90409</v>
       </c>
       <c r="E80" t="n">
-        <v>0.05898984289841098</v>
+        <v>0.2149601863659308</v>
       </c>
       <c r="F80" t="n">
-        <v>16.95207091366804</v>
+        <v>4.652024251121931</v>
       </c>
       <c r="G80" t="n">
-        <v>0.3119499239662767</v>
+        <v>0.945593236818793</v>
       </c>
       <c r="H80" t="n">
-        <v>0.09510378102295529</v>
+        <v>0.05139908706366907</v>
       </c>
       <c r="M80" t="n">
-        <v>0.02006812397972829</v>
+        <v>0.0007303119742236975</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,6007;0,3993</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>273.15</v>
+        <v>679.98</v>
       </c>
       <c r="C81" t="n">
-        <v>131.7</v>
+        <v>252.01</v>
       </c>
       <c r="D81" t="n">
-        <v>16.31321370309951</v>
+        <v>4.89885</v>
       </c>
       <c r="E81" t="n">
-        <v>0.05689837164901108</v>
+        <v>0.2142518880096612</v>
       </c>
       <c r="F81" t="n">
-        <v>17.57519540574375</v>
+        <v>4.667403444094304</v>
       </c>
       <c r="G81" t="n">
-        <v>0.3299516084400422</v>
+        <v>0.9550192703601913</v>
       </c>
       <c r="H81" t="n">
-        <v>0.07735947837209181</v>
+        <v>0.04724507913197926</v>
       </c>
       <c r="M81" t="n">
-        <v>0.01474627609082269</v>
+        <v>0.0006157184855242386</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>0,34;0,66</t>
+          <t>0,6007;0,3993</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>273.15</v>
+        <v>698.23</v>
       </c>
       <c r="C82" t="n">
-        <v>143.2</v>
+        <v>261.79</v>
       </c>
       <c r="D82" t="n">
-        <v>16.86340640809443</v>
+        <v>4.8936</v>
       </c>
       <c r="E82" t="n">
-        <v>0.05524075549964787</v>
+        <v>0.213739830693327</v>
       </c>
       <c r="F82" t="n">
-        <v>18.10257645745584</v>
+        <v>4.678585160080883</v>
       </c>
       <c r="G82" t="n">
-        <v>0.3483110598123746</v>
+        <v>0.9638420098732762</v>
       </c>
       <c r="H82" t="n">
-        <v>0.07348278392713155</v>
+        <v>0.04393796794162118</v>
       </c>
       <c r="M82" t="n">
-        <v>0.014217985289207</v>
+        <v>0.0005313951883384332</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>273.15</v>
+        <v>652.7</v>
       </c>
       <c r="C83" t="n">
-        <v>25.6</v>
+        <v>270.33</v>
       </c>
       <c r="D83" t="n">
-        <v>1.319261213720317</v>
+        <v>6.04772</v>
       </c>
       <c r="E83" t="n">
-        <v>0.7534061000247699</v>
+        <v>0.1946187100325545</v>
       </c>
       <c r="F83" t="n">
-        <v>1.327305419968225</v>
+        <v>5.138252122998486</v>
       </c>
       <c r="G83" t="n">
-        <v>0.8492464393095716</v>
+        <v>0.9694626086412045</v>
       </c>
       <c r="H83" t="n">
-        <v>0.006097508335914789</v>
+        <v>0.1503819417898835</v>
       </c>
       <c r="M83" t="n">
-        <v>5.991597607304929e-07</v>
+        <v>0.00950726229077749</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>273.15</v>
+        <v>661.85</v>
       </c>
       <c r="C84" t="n">
-        <v>33.3</v>
+        <v>277.23</v>
       </c>
       <c r="D84" t="n">
-        <v>1.801801801801802</v>
+        <v>6.0445</v>
       </c>
       <c r="E84" t="n">
-        <v>0.5444374189195926</v>
+        <v>0.1934035827343461</v>
       </c>
       <c r="F84" t="n">
-        <v>1.836758395454242</v>
+        <v>5.170535032815669</v>
       </c>
       <c r="G84" t="n">
-        <v>0.7982829196771598</v>
+        <v>0.9743410691456861</v>
       </c>
       <c r="H84" t="n">
-        <v>0.0194009094771045</v>
+        <v>0.1445884634269719</v>
       </c>
       <c r="M84" t="n">
-        <v>1.131447629427634e-05</v>
+        <v>0.008779480044431149</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>273.15</v>
+        <v>670.98</v>
       </c>
       <c r="C85" t="n">
-        <v>40.9</v>
+        <v>284.02</v>
       </c>
       <c r="D85" t="n">
-        <v>2.352941176470588</v>
+        <v>6.04126</v>
       </c>
       <c r="E85" t="n">
-        <v>0.4131502060900532</v>
+        <v>0.192315476154123</v>
       </c>
       <c r="F85" t="n">
-        <v>2.420427208457044</v>
+        <v>5.199789533311365</v>
       </c>
       <c r="G85" t="n">
-        <v>0.7440393743414763</v>
+        <v>0.9790828070767867</v>
       </c>
       <c r="H85" t="n">
-        <v>0.02868156359424374</v>
+        <v>0.1392872458210101</v>
       </c>
       <c r="M85" t="n">
-        <v>4.217004178960133e-05</v>
+        <v>0.008138764900105632</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>273.15</v>
+        <v>680.16</v>
       </c>
       <c r="C86" t="n">
-        <v>48.6</v>
+        <v>290.75</v>
       </c>
       <c r="D86" t="n">
-        <v>2.985074626865671</v>
+        <v>6.03801</v>
       </c>
       <c r="E86" t="n">
-        <v>0.3193987154603199</v>
+        <v>0.1913365502991855</v>
       </c>
       <c r="F86" t="n">
-        <v>3.130882973523522</v>
+        <v>5.226392962747258</v>
       </c>
       <c r="G86" t="n">
-        <v>0.683493000791275</v>
+        <v>0.9837220754047827</v>
       </c>
       <c r="H86" t="n">
-        <v>0.0488457961303801</v>
+        <v>0.1344179683791087</v>
       </c>
       <c r="M86" t="n">
-        <v>0.0001968525366212598</v>
+        <v>0.007571519714470337</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>273.15</v>
+        <v>689.03</v>
       </c>
       <c r="C87" t="n">
-        <v>56.2</v>
+        <v>297.17</v>
       </c>
       <c r="D87" t="n">
-        <v>3.759398496240602</v>
+        <v>6.03485</v>
       </c>
       <c r="E87" t="n">
-        <v>0.2486434741725295</v>
+        <v>0.190484985721942</v>
       </c>
       <c r="F87" t="n">
-        <v>4.021822826148725</v>
+        <v>5.249757592232163</v>
       </c>
       <c r="G87" t="n">
-        <v>0.6152873950005056</v>
+        <v>0.9880829940543671</v>
       </c>
       <c r="H87" t="n">
-        <v>0.06980487175556079</v>
+        <v>0.1300931104779469</v>
       </c>
       <c r="M87" t="n">
-        <v>0.0006376530456271067</v>
+        <v>0.007084713663617253</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0,349;0,651</t>
+          <t>0,6761;0,3239</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>273.15</v>
+        <v>698.3099999999999</v>
       </c>
       <c r="C88" t="n">
-        <v>66.40000000000001</v>
+        <v>303.82</v>
       </c>
       <c r="D88" t="n">
-        <v>5.128205128205128</v>
+        <v>6.03154</v>
       </c>
       <c r="E88" t="n">
-        <v>0.1700614851194655</v>
+        <v>0.1896730148836821</v>
       </c>
       <c r="F88" t="n">
-        <v>5.880226197586806</v>
+        <v>5.272231269235926</v>
       </c>
       <c r="G88" t="n">
-        <v>0.4972086596052916</v>
+        <v>0.9925205042862572</v>
       </c>
       <c r="H88" t="n">
-        <v>0.1466441085294273</v>
+        <v>0.1258896949641508</v>
       </c>
       <c r="M88" t="n">
-        <v>0.005236441562907064</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>0,349;0,651</t>
-        </is>
-      </c>
-      <c r="B89" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C89" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="D89" t="n">
-        <v>6.289308176100628</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0.1214917553866694</v>
-      </c>
-      <c r="F89" t="n">
-        <v>8.231011205800097</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0.3878371892991083</v>
-      </c>
-      <c r="H89" t="n">
-        <v>0.3087307817222156</v>
-      </c>
-      <c r="M89" t="n">
-        <v>0.0349093579217046</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B90" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C90" t="n">
-        <v>29.5</v>
-      </c>
-      <c r="D90" t="n">
-        <v>1.533742331288344</v>
-      </c>
-      <c r="E90" t="n">
-        <v>0.6421890355706589</v>
-      </c>
-      <c r="F90" t="n">
-        <v>1.557173892125681</v>
-      </c>
-      <c r="G90" t="n">
-        <v>0.8341603437200138</v>
-      </c>
-      <c r="H90" t="n">
-        <v>0.01527737766594372</v>
-      </c>
-      <c r="M90" t="n">
-        <v>5.083685585868748e-06</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B91" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C91" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="D91" t="n">
-        <v>1.773049645390071</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0.5528084002229667</v>
-      </c>
-      <c r="F91" t="n">
-        <v>1.808945015301261</v>
-      </c>
-      <c r="G91" t="n">
-        <v>0.8105568949095773</v>
-      </c>
-      <c r="H91" t="n">
-        <v>0.02024498862991098</v>
-      </c>
-      <c r="M91" t="n">
-        <v>1.193034797278835e-05</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C92" t="n">
-        <v>40.9</v>
-      </c>
-      <c r="D92" t="n">
-        <v>2.298850574712644</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0.4226439481304881</v>
-      </c>
-      <c r="F92" t="n">
-        <v>2.366057776110064</v>
-      </c>
-      <c r="G92" t="n">
-        <v>0.7611365893102735</v>
-      </c>
-      <c r="H92" t="n">
-        <v>0.02923513260787803</v>
-      </c>
-      <c r="M92" t="n">
-        <v>4.182229555253218e-05</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C93" t="n">
-        <v>48.6</v>
-      </c>
-      <c r="D93" t="n">
-        <v>2.890173410404624</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.3305275139370112</v>
-      </c>
-      <c r="F93" t="n">
-        <v>3.025466739784243</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0.7073079239511023</v>
-      </c>
-      <c r="H93" t="n">
-        <v>0.04681149196534787</v>
-      </c>
-      <c r="M93" t="n">
-        <v>0.0001694841201353874</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C94" t="n">
-        <v>66.40000000000001</v>
-      </c>
-      <c r="D94" t="n">
-        <v>4.716981132075472</v>
-      </c>
-      <c r="E94" t="n">
-        <v>0.191314861548767</v>
-      </c>
-      <c r="F94" t="n">
-        <v>5.226985462104812</v>
-      </c>
-      <c r="G94" t="n">
-        <v>0.5593471432194754</v>
-      </c>
-      <c r="H94" t="n">
-        <v>0.1081209179662201</v>
-      </c>
-      <c r="M94" t="n">
-        <v>0.002408374228228483</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C95" t="n">
-        <v>85.59999999999999</v>
-      </c>
-      <c r="D95" t="n">
-        <v>8</v>
-      </c>
-      <c r="E95" t="n">
-        <v>0.09621899193876575</v>
-      </c>
-      <c r="F95" t="n">
-        <v>10.39295860256367</v>
-      </c>
-      <c r="G95" t="n">
-        <v>0.3626596218988642</v>
-      </c>
-      <c r="H95" t="n">
-        <v>0.2991198253204588</v>
-      </c>
-      <c r="M95" t="n">
-        <v>0.0530208414220692</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C96" t="n">
-        <v>104.7</v>
-      </c>
-      <c r="D96" t="n">
-        <v>11.73708920187793</v>
-      </c>
-      <c r="E96" t="n">
-        <v>0.07200674635604731</v>
-      </c>
-      <c r="F96" t="n">
-        <v>13.88758763040565</v>
-      </c>
-      <c r="G96" t="n">
-        <v>0.331959044977356</v>
-      </c>
-      <c r="H96" t="n">
-        <v>0.1832224661105616</v>
-      </c>
-      <c r="M96" t="n">
-        <v>0.04282077306574249</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C97" t="n">
-        <v>120.1</v>
-      </c>
-      <c r="D97" t="n">
-        <v>13.6986301369863</v>
-      </c>
-      <c r="E97" t="n">
-        <v>0.06518874784117989</v>
-      </c>
-      <c r="F97" t="n">
-        <v>15.34007068882979</v>
-      </c>
-      <c r="G97" t="n">
-        <v>0.3447309559297137</v>
-      </c>
-      <c r="H97" t="n">
-        <v>0.1198251602845746</v>
-      </c>
-      <c r="M97" t="n">
-        <v>0.02494747301144679</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C98" t="n">
-        <v>127.8</v>
-      </c>
-      <c r="D98" t="n">
-        <v>14.28571428571428</v>
-      </c>
-      <c r="E98" t="n">
-        <v>0.06291491376218883</v>
-      </c>
-      <c r="F98" t="n">
-        <v>15.89448256704103</v>
-      </c>
-      <c r="G98" t="n">
-        <v>0.3540373624454325</v>
-      </c>
-      <c r="H98" t="n">
-        <v>0.112613779692872</v>
-      </c>
-      <c r="M98" t="n">
-        <v>0.02396421650928705</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>0,408;0,592</t>
-        </is>
-      </c>
-      <c r="B99" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C99" t="n">
-        <v>143.2</v>
-      </c>
-      <c r="D99" t="n">
-        <v>15.36098310291859</v>
-      </c>
-      <c r="E99" t="n">
-        <v>0.05949976041607968</v>
-      </c>
-      <c r="F99" t="n">
-        <v>16.80679036364241</v>
-      </c>
-      <c r="G99" t="n">
-        <v>0.3751654810231405</v>
-      </c>
-      <c r="H99" t="n">
-        <v>0.09412205267312077</v>
-      </c>
-      <c r="M99" t="n">
-        <v>0.01935517254779371</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B100" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C100" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="D100" t="n">
-        <v>1.182033096926714</v>
-      </c>
-      <c r="E100" t="n">
-        <v>0.8364967914953465</v>
-      </c>
-      <c r="F100" t="n">
-        <v>1.195461847752423</v>
-      </c>
-      <c r="G100" t="n">
-        <v>0.8802921267839673</v>
-      </c>
-      <c r="H100" t="n">
-        <v>0.01136072319854976</v>
-      </c>
-      <c r="M100" t="n">
-        <v>1.669734710546097e-06</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B101" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C101" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D101" t="n">
-        <v>1.721170395869191</v>
-      </c>
-      <c r="E101" t="n">
-        <v>0.5681024366610473</v>
-      </c>
-      <c r="F101" t="n">
-        <v>1.760245926557502</v>
-      </c>
-      <c r="G101" t="n">
-        <v>0.8304803725908658</v>
-      </c>
-      <c r="H101" t="n">
-        <v>0.02270288332990885</v>
-      </c>
-      <c r="M101" t="n">
-        <v>1.413793609789959e-05</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B102" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C102" t="n">
-        <v>40.9</v>
-      </c>
-      <c r="D102" t="n">
-        <v>2.207505518763797</v>
-      </c>
-      <c r="E102" t="n">
-        <v>0.4372822765025689</v>
-      </c>
-      <c r="F102" t="n">
-        <v>2.286852346264999</v>
-      </c>
-      <c r="G102" t="n">
-        <v>0.7874986545418083</v>
-      </c>
-      <c r="H102" t="n">
-        <v>0.03594411285804488</v>
-      </c>
-      <c r="M102" t="n">
-        <v>5.829554661579292e-05</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B103" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C103" t="n">
-        <v>48.5</v>
-      </c>
-      <c r="D103" t="n">
-        <v>2.73972602739726</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0.3480521616558207</v>
-      </c>
-      <c r="F103" t="n">
-        <v>2.873132565080497</v>
-      </c>
-      <c r="G103" t="n">
-        <v>0.7432770290271485</v>
-      </c>
-      <c r="H103" t="n">
-        <v>0.04869338625438149</v>
-      </c>
-      <c r="M103" t="n">
-        <v>0.0001647898545984159</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B104" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C104" t="n">
-        <v>66.40000000000001</v>
-      </c>
-      <c r="D104" t="n">
-        <v>4.237288135593221</v>
-      </c>
-      <c r="E104" t="n">
-        <v>0.2157390785795113</v>
-      </c>
-      <c r="F104" t="n">
-        <v>4.635228844881929</v>
-      </c>
-      <c r="G104" t="n">
-        <v>0.6307562115528148</v>
-      </c>
-      <c r="H104" t="n">
-        <v>0.09391400739213528</v>
-      </c>
-      <c r="M104" t="n">
-        <v>0.001466266741751858</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B105" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C105" t="n">
-        <v>85.59999999999999</v>
-      </c>
-      <c r="D105" t="n">
-        <v>6.451612903225807</v>
-      </c>
-      <c r="E105" t="n">
-        <v>0.1332447025583772</v>
-      </c>
-      <c r="F105" t="n">
-        <v>7.504988797298561</v>
-      </c>
-      <c r="G105" t="n">
-        <v>0.5022134661377492</v>
-      </c>
-      <c r="H105" t="n">
-        <v>0.1632732635812769</v>
-      </c>
-      <c r="M105" t="n">
-        <v>0.01027408124271828</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B106" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C106" t="n">
-        <v>104.7</v>
-      </c>
-      <c r="D106" t="n">
-        <v>9.090909090909092</v>
-      </c>
-      <c r="E106" t="n">
-        <v>0.0917847100932781</v>
-      </c>
-      <c r="F106" t="n">
-        <v>10.89506083293971</v>
-      </c>
-      <c r="G106" t="n">
-        <v>0.4231376398460091</v>
-      </c>
-      <c r="H106" t="n">
-        <v>0.1984566916233677</v>
-      </c>
-      <c r="M106" t="n">
-        <v>0.03013855100251949</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B107" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C107" t="n">
-        <v>112.4</v>
-      </c>
-      <c r="D107" t="n">
-        <v>10.11122345803842</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0.08354306043374733</v>
-      </c>
-      <c r="F107" t="n">
-        <v>11.96987511360128</v>
-      </c>
-      <c r="G107" t="n">
-        <v>0.413467453314158</v>
-      </c>
-      <c r="H107" t="n">
-        <v>0.1838206487351668</v>
-      </c>
-      <c r="M107" t="n">
-        <v>0.03198690719191256</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B108" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C108" t="n">
-        <v>127.8</v>
-      </c>
-      <c r="D108" t="n">
-        <v>11.97604790419162</v>
-      </c>
-      <c r="E108" t="n">
-        <v>0.07347319610490882</v>
-      </c>
-      <c r="F108" t="n">
-        <v>13.61040560386332</v>
-      </c>
-      <c r="G108" t="n">
-        <v>0.4134513584130672</v>
-      </c>
-      <c r="H108" t="n">
-        <v>0.1364688679225877</v>
-      </c>
-      <c r="M108" t="n">
-        <v>0.02473263972663147</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>0,508;0,492</t>
-        </is>
-      </c>
-      <c r="B109" t="n">
-        <v>273.15</v>
-      </c>
-      <c r="C109" t="n">
-        <v>143.2</v>
-      </c>
-      <c r="D109" t="n">
-        <v>13.35113484646195</v>
-      </c>
-      <c r="E109" t="n">
-        <v>0.06749066525569894</v>
-      </c>
-      <c r="F109" t="n">
-        <v>14.81686387608336</v>
-      </c>
-      <c r="G109" t="n">
-        <v>0.4255507537872931</v>
-      </c>
-      <c r="H109" t="n">
-        <v>0.1097831043186438</v>
-      </c>
-      <c r="M109" t="n">
-        <v>0.01989223692847155</v>
+        <v>0.006627008604764931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>